<commit_message>
Updated the list of the electonic components
</commit_message>
<xml_diff>
--- a/doc/analyse/VermogenLijstElektrischeComponenten.xlsx
+++ b/doc/analyse/VermogenLijstElektrischeComponenten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gener\Desktop\Mappen\School\3de jaar (2018-2019)\Internet Of Things\iot18-LF1\doc\analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\AP\iot1819--iot18lf1\doc\analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F687836-F417-4AA1-AFF3-17D436C524E0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04EB316-7D24-42A9-9B28-6DCFAE5CD135}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{2F75D7C5-6928-426A-81CA-4210FB250206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7488" xr2:uid="{2F75D7C5-6928-426A-81CA-4210FB250206}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="26">
   <si>
     <t>Temperature Sensor</t>
   </si>
@@ -93,14 +93,32 @@
     <t>Raspberry Pi</t>
   </si>
   <si>
-    <t>TODO: MOTOR CONTROLLER + PUMP CONTROLLER</t>
+    <t>A3967 Easydriver</t>
+  </si>
+  <si>
+    <t>42BYGHM809 StepperMotor</t>
+  </si>
+  <si>
+    <t>QR30E (pomp)</t>
+  </si>
+  <si>
+    <t>SHURflo 355-100-00 (pomp)</t>
+  </si>
+  <si>
+    <t>Totaal</t>
+  </si>
+  <si>
+    <t>Stroom(Typ.) (A)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,14 +148,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,14 +184,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -211,6 +217,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -218,7 +310,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
@@ -226,12 +318,26 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Goed" xfId="2" builtinId="26"/>
@@ -555,38 +661,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06C285C-C858-497A-8CA6-C24776171F2C}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I2"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="9" max="9" width="76" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -602,12 +702,8 @@
       <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -625,7 +721,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -643,16 +739,16 @@
         <v>5.9999999999999995E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:5" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -669,7 +765,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
         <f>A3</f>
         <v>Attiny 85</v>
@@ -691,16 +787,16 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -717,7 +813,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="str">
         <f>A7</f>
         <v>Attiny 85</v>
@@ -739,7 +835,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -757,16 +853,16 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
@@ -783,7 +879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="str">
         <f>A10</f>
         <v>Attiny 85</v>
@@ -805,7 +901,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -823,16 +919,16 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
@@ -849,7 +945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -867,7 +963,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
@@ -885,7 +981,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
@@ -903,7 +999,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
@@ -921,131 +1017,377 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+    <row r="23" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="3">
+        <v>5</v>
+      </c>
+      <c r="C25" s="6">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3">
+        <v>12</v>
+      </c>
+      <c r="E25" s="6">
+        <f>D25*B25/1000</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="3">
+        <v>5</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" ref="E26" si="1">D26*B26/1000</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3">
+        <v>5</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" ref="E27:E28" si="2">D27*B27/1000</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="3">
+        <v>5</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="2"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="3">
+        <v>12</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1700</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="6">
+        <f>C29*B29/1000</f>
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="3">
+        <v>12</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1700</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" ref="E30:E31" si="3">C30*B30/1000</f>
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="3">
+        <v>12</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1700</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="3"/>
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="3">
+        <v>5</v>
+      </c>
+      <c r="C34" s="6">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3">
+        <v>12</v>
+      </c>
+      <c r="E34" s="6">
+        <f>D34*B34/1000</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="3">
+        <v>12</v>
+      </c>
+      <c r="C35" s="6">
+        <v>3750</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="6">
+        <f>C35*B35/1000</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="3">
+        <v>12</v>
+      </c>
+      <c r="C36" s="6">
+        <v>350</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="6">
+        <f>C36*B36/1000</f>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>19</v>
       </c>
-      <c r="B31">
+      <c r="B39">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C31">
+      <c r="C39">
         <v>1250</v>
       </c>
-      <c r="D31">
+      <c r="D39">
         <v>2500</v>
       </c>
-      <c r="E31">
-        <f>D31*B31/1000</f>
+      <c r="E39">
+        <f>D39*B39/1000</f>
         <v>12.75</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>19</v>
       </c>
-      <c r="B32">
+      <c r="B40">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C32">
+      <c r="C40">
         <v>1250</v>
       </c>
-      <c r="D32">
+      <c r="D40">
         <v>2500</v>
       </c>
-      <c r="E32">
-        <f t="shared" ref="E32:E34" si="1">D32*B32/1000</f>
+      <c r="E40">
+        <f t="shared" ref="E40:E42" si="4">D40*B40/1000</f>
         <v>12.75</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>19</v>
       </c>
-      <c r="B33">
+      <c r="B41">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C33">
+      <c r="C41">
         <v>1250</v>
       </c>
-      <c r="D33">
+      <c r="D41">
         <v>2500</v>
       </c>
-      <c r="E33">
-        <f t="shared" si="1"/>
+      <c r="E41">
+        <f t="shared" si="4"/>
         <v>12.75</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>19</v>
       </c>
-      <c r="B34">
+      <c r="B42">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C34">
+      <c r="C42">
         <v>1250</v>
       </c>
-      <c r="D34">
+      <c r="D42">
         <v>2500</v>
       </c>
-      <c r="E34">
-        <f t="shared" si="1"/>
+      <c r="E42">
+        <f t="shared" si="4"/>
         <v>12.75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="11"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="15"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="17">
+        <f>SUM(C39:C42,C34:C36,C25:C31,C18:C21,C14:C15,C10:C11,C7,C3:C4)/1000</f>
+        <v>19.575009000000001</v>
+      </c>
+      <c r="D46" s="16"/>
+      <c r="E46" s="18">
+        <f>SUM(E39:E42,E34:E36,E25:E31,E18:E21,E14:E15,E10:E11,E7,E3:E4)</f>
+        <v>214.77035999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A44:E44"/>
     <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A32:E32"/>
     <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="F1:I2"/>
+    <mergeCell ref="A37:E37"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A12:E12"/>
@@ -1053,5 +1395,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E29 E35" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>